<commit_message>
Got to fix variable choosing in log() step
</commit_message>
<xml_diff>
--- a/Project-Functions.xlsx
+++ b/Project-Functions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>t1 + t2</t>
   </si>
   <si>
     <t>t1</t>
@@ -321,7 +324,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -596,6 +599,9 @@
       <c r="C15" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="D15" s="0" t="s">
+        <v>37</v>
+      </c>
       <c r="F15" s="0" t="n">
         <v>0</v>
       </c>
@@ -608,10 +614,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>1</v>
@@ -625,10 +631,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>1</v>
@@ -642,10 +648,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>1</v>
@@ -659,10 +665,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>1</v>
@@ -676,10 +682,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>1</v>
@@ -693,10 +699,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>1</v>
@@ -710,10 +716,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>1</v>
@@ -727,10 +733,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>1</v>
@@ -744,10 +750,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>1</v>
@@ -761,10 +767,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>1</v>
@@ -778,7 +784,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>

</xml_diff>